<commit_message>
Added 7-18-19 SubCh1 Submission
</commit_message>
<xml_diff>
--- a/SubChallenge2/submission/submission_7-11-19/SubmissionWorksheet.xlsx
+++ b/SubChallenge2/submission/submission_7-11-19/SubmissionWorksheet.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby Ford\Desktop\malaria_DREAM2019\SubChallenge2\submission\submission_7-11-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327336A-7B13-4341-89F0-6F141E3699EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1426C39-7384-4885-BA68-49FC448205E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A39D8EA-6F43-43C7-9B99-F166BEA2F3FD}"/>
+    <workbookView xWindow="7095" yWindow="3600" windowWidth="19755" windowHeight="11385" xr2:uid="{1A39D8EA-6F43-43C7-9B99-F166BEA2F3FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="46">
   <si>
     <t>Isolate</t>
   </si>
@@ -170,6 +170,9 @@
   <si>
     <t>Min of Probability_0</t>
   </si>
+  <si>
+    <t>Average of Prediction2</t>
+  </si>
 </sst>
 </file>
 
@@ -2313,8 +2316,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1F7AD34-3329-48FD-863E-AF0A7EFFC19F}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G1:I34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1F7AD34-3329-48FD-863E-AF0A7EFFC19F}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G1:J34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
       <items count="33">
@@ -2465,16 +2468,20 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="3">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
   </colItems>
-  <dataFields count="2">
+  <dataFields count="3">
     <dataField name="Sum of Prediction" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Average of Prediction2" fld="1" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Min of Probability_0" fld="2" subtotal="min" baseField="0" baseItem="2"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -2788,8 +2795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4952C8D-FBF0-419F-993B-04FBEEF47BD6}">
   <dimension ref="A1:N289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,8 +2806,9 @@
     <col min="3" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2828,6 +2836,9 @@
         <v>36</v>
       </c>
       <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
         <v>44</v>
       </c>
       <c r="L1" t="s">
@@ -2863,9 +2874,11 @@
         <v>0</v>
       </c>
       <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
         <v>0.49727167999999999</v>
       </c>
-      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="2" t="s">
         <v>1</v>
@@ -2900,9 +2913,11 @@
         <v>0</v>
       </c>
       <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
         <v>0.58482548999999995</v>
       </c>
-      <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="2" t="s">
         <v>2</v>
@@ -2937,9 +2952,11 @@
         <v>0</v>
       </c>
       <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
         <v>0.65407694999999999</v>
       </c>
-      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="2" t="s">
         <v>3</v>
@@ -2974,9 +2991,11 @@
         <v>0</v>
       </c>
       <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
         <v>0.65200411000000003</v>
       </c>
-      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="2" t="s">
         <v>4</v>
@@ -3011,9 +3030,11 @@
         <v>0</v>
       </c>
       <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
         <v>0.64158674999999998</v>
       </c>
-      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="2" t="s">
         <v>5</v>
@@ -3048,9 +3069,11 @@
         <v>0</v>
       </c>
       <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
         <v>0.54473621999999999</v>
       </c>
-      <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="2" t="s">
         <v>6</v>
@@ -3085,9 +3108,11 @@
         <v>0</v>
       </c>
       <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
         <v>0.52077134999999997</v>
       </c>
-      <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="2" t="s">
         <v>7</v>
@@ -3122,9 +3147,11 @@
         <v>0</v>
       </c>
       <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
         <v>0.59652888000000004</v>
       </c>
-      <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="2" t="s">
         <v>8</v>
@@ -3159,9 +3186,11 @@
         <v>0</v>
       </c>
       <c r="I10" s="3">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
         <v>0.56491265000000002</v>
       </c>
-      <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2" t="s">
         <v>9</v>
@@ -3196,9 +3225,11 @@
         <v>1</v>
       </c>
       <c r="I11" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="J11" s="3">
         <v>0.36864523999999999</v>
       </c>
-      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="2" t="s">
         <v>10</v>
@@ -3233,9 +3264,11 @@
         <v>1</v>
       </c>
       <c r="I12" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="J12" s="3">
         <v>0.42320065000000001</v>
       </c>
-      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="2" t="s">
         <v>11</v>
@@ -3270,9 +3303,11 @@
         <v>0</v>
       </c>
       <c r="I13" s="3">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
         <v>0.64491145999999999</v>
       </c>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="2" t="s">
         <v>12</v>
@@ -3307,9 +3342,11 @@
         <v>0</v>
       </c>
       <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
         <v>0.58171421999999995</v>
       </c>
-      <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="2" t="s">
         <v>13</v>
@@ -3344,9 +3381,11 @@
         <v>0</v>
       </c>
       <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
         <v>0.54046727999999999</v>
       </c>
-      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="2" t="s">
         <v>14</v>
@@ -3381,9 +3420,11 @@
         <v>0</v>
       </c>
       <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
         <v>0.52546565999999995</v>
       </c>
-      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="2" t="s">
         <v>15</v>
@@ -3418,9 +3459,11 @@
         <v>0</v>
       </c>
       <c r="I17" s="3">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
         <v>0.49652846</v>
       </c>
-      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="2" t="s">
         <v>16</v>
@@ -3455,9 +3498,11 @@
         <v>0</v>
       </c>
       <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
         <v>0.44627994999999998</v>
       </c>
-      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="2" t="s">
         <v>17</v>
@@ -3492,9 +3537,11 @@
         <v>0</v>
       </c>
       <c r="I19" s="3">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
         <v>0.51708012999999997</v>
       </c>
-      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="2" t="s">
         <v>18</v>
@@ -3529,9 +3576,11 @@
         <v>1</v>
       </c>
       <c r="I20" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="J20" s="3">
         <v>0.43375606999999999</v>
       </c>
-      <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="2" t="s">
         <v>19</v>
@@ -3566,9 +3615,11 @@
         <v>1</v>
       </c>
       <c r="I21" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="J21" s="3">
         <v>0.47079870000000001</v>
       </c>
-      <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="2" t="s">
         <v>20</v>
@@ -3603,9 +3654,11 @@
         <v>0</v>
       </c>
       <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
         <v>0.64371694000000002</v>
       </c>
-      <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="2" t="s">
         <v>21</v>
@@ -3640,9 +3693,11 @@
         <v>2</v>
       </c>
       <c r="I23" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J23" s="3">
         <v>0.39759166000000001</v>
       </c>
-      <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="2" t="s">
         <v>22</v>
@@ -3677,9 +3732,11 @@
         <v>0</v>
       </c>
       <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
         <v>0.49415889000000002</v>
       </c>
-      <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="2" t="s">
         <v>23</v>
@@ -3714,9 +3771,11 @@
         <v>0</v>
       </c>
       <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
         <v>0.56173368000000001</v>
       </c>
-      <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="2" t="s">
         <v>24</v>
@@ -3751,9 +3810,11 @@
         <v>0</v>
       </c>
       <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
         <v>0.58218800999999998</v>
       </c>
-      <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="2" t="s">
         <v>25</v>
@@ -3788,9 +3849,11 @@
         <v>0</v>
       </c>
       <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
         <v>0.62843749999999998</v>
       </c>
-      <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="2" t="s">
         <v>26</v>
@@ -3825,9 +3888,11 @@
         <v>0</v>
       </c>
       <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
         <v>0.58425278999999997</v>
       </c>
-      <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="2" t="s">
         <v>27</v>
@@ -3862,9 +3927,11 @@
         <v>0</v>
       </c>
       <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
         <v>0.56505285999999999</v>
       </c>
-      <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="2" t="s">
         <v>28</v>
@@ -3899,9 +3966,11 @@
         <v>2</v>
       </c>
       <c r="I30" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J30" s="3">
         <v>0.44200781</v>
       </c>
-      <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="2" t="s">
         <v>29</v>
@@ -3936,9 +4005,11 @@
         <v>0</v>
       </c>
       <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
         <v>0.59823256999999996</v>
       </c>
-      <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="2" t="s">
         <v>30</v>
@@ -3973,9 +4044,11 @@
         <v>1</v>
       </c>
       <c r="I32" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="J32" s="3">
         <v>0.46708696999999999</v>
       </c>
-      <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="2" t="s">
         <v>31</v>
@@ -4010,9 +4083,11 @@
         <v>0</v>
       </c>
       <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
         <v>0.62649157</v>
       </c>
-      <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="2" t="s">
         <v>32</v>
@@ -4047,9 +4122,11 @@
         <v>9</v>
       </c>
       <c r="I34" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J34" s="3">
         <v>0.36864523999999999</v>
       </c>
-      <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>